<commit_message>
now adding features for using existing and new files
</commit_message>
<xml_diff>
--- a/ExcelOps/bookxml.xlsx
+++ b/ExcelOps/bookxml.xlsx
@@ -7,12 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="sheet2" r:id="rId4" sheetId="2"/>
+    <sheet name="sheet4" r:id="rId5" sheetId="3"/>
+    <sheet name="sheet6" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>rollno</t>
   </si>
@@ -106,10 +109,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -118,7 +121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
@@ -199,4 +202,76 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>